<commit_message>
Finaliza programacion del ejemplo 1 de la regla El Jugador 1 comienza en la posición
</commit_message>
<xml_diff>
--- a/docs/battleground.xlsx
+++ b/docs/battleground.xlsx
@@ -398,194 +398,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:X17"/>
+  <dimension ref="C2:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="5.77734375" style="2" customWidth="1"/>
-    <col min="5" max="12" width="5.77734375" customWidth="1"/>
-    <col min="13" max="13" width="5.77734375" style="4" customWidth="1"/>
-    <col min="14" max="20" width="5.77734375" customWidth="1"/>
-    <col min="23" max="23" width="5.77734375" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" style="2" customWidth="1"/>
+    <col min="4" max="11" width="5.77734375" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" style="4" customWidth="1"/>
+    <col min="13" max="19" width="5.77734375" customWidth="1"/>
+    <col min="22" max="22" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="H2" s="2" t="s">
+    <row r="2" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="4:24" s="2" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
+    <row r="3" spans="3:23" s="2" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="2">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="5" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2">
-        <v>2</v>
-      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="6" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
-        <v>3</v>
-      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="2">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="7" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>4</v>
-      </c>
-      <c r="N7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="8" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2">
-        <v>5</v>
-      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
+        <v>4</v>
+      </c>
+      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="2">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="9" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2">
-        <v>6</v>
-      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2">
+        <v>5</v>
+      </c>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="4:24" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="2">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="10" spans="3:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2">
-        <v>7</v>
-      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2">
+        <v>6</v>
+      </c>
+      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="4:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
       <c r="E11" s="2">
         <v>1</v>
       </c>
@@ -604,11 +607,11 @@
       <c r="J11" s="2">
         <v>6</v>
       </c>
-      <c r="K11" s="2">
-        <v>7</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="5"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
       <c r="N11" s="2">
         <v>1</v>
       </c>
@@ -627,28 +630,25 @@
       <c r="S11" s="2">
         <v>6</v>
       </c>
-      <c r="T11" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="W15" s="6"/>
-      <c r="X15" t="s">
+    </row>
+    <row r="12" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="V15" s="6"/>
+      <c r="W15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W17" s="7"/>
-      <c r="X17" t="s">
+    <row r="17" spans="22:23" x14ac:dyDescent="0.3">
+      <c r="V17" s="7"/>
+      <c r="W17" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
avance edu zona de busqueda
</commit_message>
<xml_diff>
--- a/docs/battleground.xlsx
+++ b/docs/battleground.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="está_empezando_el_juego" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ZONA DE BUSQUEDA DE JUGADOR 1</t>
   </si>
@@ -31,13 +32,40 @@
   </si>
   <si>
     <t>BUFF ATAQUE</t>
+  </si>
+  <si>
+    <t>está_empezando_el_juego</t>
+  </si>
+  <si>
+    <t>Iniciar Zona de Busqueda</t>
+  </si>
+  <si>
+    <t>Cargar ArrayList de 7x7</t>
+  </si>
+  <si>
+    <t>Cargar Buff en las posiciones del Array List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cargar Player en la Posicion </t>
+  </si>
+  <si>
+    <t>(Esperar/Cargar) Lista de Movimientos de Player</t>
+  </si>
+  <si>
+    <t>Ejecutar Lista de Movimientos</t>
+  </si>
+  <si>
+    <t>Realizar Busqueda</t>
+  </si>
+  <si>
+    <t>por cada movimiento chequear casillero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,8 +73,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFC66D"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +127,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -102,10 +163,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -118,8 +180,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -133,6 +207,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9001125" y="238125"/>
+          <a:ext cx="3057525" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,257 +532,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:W17"/>
+  <dimension ref="D2:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.77734375" style="2" customWidth="1"/>
-    <col min="4" max="11" width="5.77734375" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" style="4" customWidth="1"/>
-    <col min="13" max="19" width="5.77734375" customWidth="1"/>
-    <col min="22" max="22" width="5.77734375" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="2" customWidth="1"/>
+    <col min="5" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="4" customWidth="1"/>
+    <col min="14" max="20" width="5.7109375" customWidth="1"/>
+    <col min="23" max="23" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="G2" s="2" t="s">
+    <row r="2" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:23" s="2" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="2">
+    <row r="3" spans="4:24" s="2" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2">
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2">
         <v>0</v>
       </c>
-      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="2">
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2">
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="2">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2">
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2">
         <v>2</v>
       </c>
-      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="2">
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2">
+      <c r="J7" s="1"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2">
         <v>3</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="3"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="2">
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2">
         <v>4</v>
       </c>
-      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="2">
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="4:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2">
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2">
         <v>5</v>
       </c>
-      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="3:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2">
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="4:24" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
         <v>6</v>
       </c>
-      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2">
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2">
         <v>6</v>
       </c>
-      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="D11" s="2">
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>2</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>3</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>4</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>5</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>6</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="2">
+      <c r="L11" s="2"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="2">
         <v>0</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>1</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <v>2</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>3</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
         <v>4</v>
       </c>
-      <c r="R11" s="2">
+      <c r="S11" s="2">
         <v>5</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="3:23" x14ac:dyDescent="0.3">
-      <c r="V15" s="6"/>
-      <c r="W15" t="s">
+    <row r="12" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="W15" s="6"/>
+      <c r="X15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="22:23" x14ac:dyDescent="0.3">
-      <c r="V17" s="7"/>
-      <c r="W17" t="s">
+    <row r="17" spans="23:24" x14ac:dyDescent="0.25">
+      <c r="W17" s="7"/>
+      <c r="X17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -656,4 +790,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B6:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>